<commit_message>
tests/integration: two Excel-related tests
</commit_message>
<xml_diff>
--- a/tests/integration/commands/export/excel/01_basic_excel_export/expected/input.xlsx
+++ b/tests/integration/commands/export/excel/01_basic_excel_export/expected/input.xlsx
@@ -1,50 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27815"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Stanislaw/workspace/projects-code/strictdoc/tests/integration/commands/export/excel/01_basic_excel_export/expected/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="requirements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Title #1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+  <si>
+    <t>REQ-001</t>
   </si>
   <si>
     <t>Statement #1</t>
   </si>
   <si>
-    <t>Title #2</t>
+    <t>REQ-002</t>
+  </si>
+  <si>
+    <t>REQ-003</t>
+  </si>
+  <si>
+    <t>Statement #3</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>STATEMENT</t>
+  </si>
+  <si>
+    <t>PARENT</t>
   </si>
   <si>
     <t>Statement #2</t>
-  </si>
-  <si>
-    <t>Title #3</t>
-  </si>
-  <si>
-    <t>Statement #3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,22 +93,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="UID"/>
+    <tableColumn id="2" name="STATEMENT"/>
+    <tableColumn id="3" name="PARENT"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -121,12 +173,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -153,14 +205,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -187,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,38 +416,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" location="'requirements'!A2" display="REQ-001"/>
+    <hyperlink ref="C4" location="'requirements'!A3" display="REQ-002"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export/excel: export special fields
</commit_message>
<xml_diff>
--- a/tests/integration/commands/export/excel/01_basic_excel_export/expected/input.xlsx
+++ b/tests/integration/commands/export/excel/01_basic_excel_export/expected/input.xlsx
@@ -1,28 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27815"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Stanislaw/workspace/projects-code/strictdoc/tests/integration/commands/export/excel/01_basic_excel_export/expected/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -38,6 +25,9 @@
     <t>REQ-002</t>
   </si>
   <si>
+    <t>Statement #2</t>
+  </si>
+  <si>
     <t>REQ-003</t>
   </si>
   <si>
@@ -51,16 +41,13 @@
   </si>
   <si>
     <t>PARENT</t>
-  </si>
-  <si>
-    <t>Statement #2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,15 +93,10 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -131,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -173,12 +155,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -205,15 +187,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -240,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,32 +396,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -449,23 +427,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -473,8 +451,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" location="'requirements'!A2" display="REQ-001"/>
-    <hyperlink ref="C4" location="'requirements'!A3" display="REQ-002"/>
+    <hyperlink ref="C3" location="'Requirements'!A2" display="REQ-001"/>
+    <hyperlink ref="C4" location="'Requirements'!A3" display="REQ-002"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>